<commit_message>
added nbstripout commit hook and updated condition assignments
</commit_message>
<xml_diff>
--- a/assignment/assignments.xlsx
+++ b/assignment/assignments.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Richer/Documents/Android/AndroidStudioProjects/CARWatch/assignment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D3530FE-80C9-FA4C-A7B6-3620E0BE6BD9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5670593-558A-524D-8E3B-07453DC3B28E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25440" windowHeight="15400" tabRatio="1000" xr2:uid="{FE598AF7-C224-4D25-8198-8A6438CC96D5}"/>
+    <workbookView xWindow="-8540" yWindow="-28340" windowWidth="51200" windowHeight="28340" tabRatio="1000" xr2:uid="{FE598AF7-C224-4D25-8198-8A6438CC96D5}"/>
   </bookViews>
   <sheets>
     <sheet name="Bedingungszuweisung" sheetId="17" r:id="rId1"/>
     <sheet name="ChronotypAuswertung_str Abend" sheetId="7" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bedingungszuweisung!$A$1:$D$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Bedingungszuweisung!$A$1:$B$107</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="292">
   <si>
     <t>Code</t>
   </si>
@@ -850,52 +850,67 @@
     <t>LS13L</t>
   </si>
   <si>
-    <t>EU25L</t>
-  </si>
-  <si>
     <t>PS06G</t>
   </si>
   <si>
     <t>JK20G</t>
   </si>
   <si>
-    <t>LU16N</t>
-  </si>
-  <si>
     <t>MC04A</t>
   </si>
   <si>
-    <t>MH17F</t>
-  </si>
-  <si>
     <t>MS28B</t>
   </si>
   <si>
-    <t>Zuweisung</t>
-  </si>
-  <si>
     <t>KL24U</t>
   </si>
   <si>
-    <t>AE01U</t>
-  </si>
-  <si>
-    <t>RB14R</t>
-  </si>
-  <si>
     <t>SE06H</t>
   </si>
   <si>
     <t>LW28E</t>
   </si>
   <si>
-    <t>AS03C</t>
-  </si>
-  <si>
     <t>IM09E</t>
   </si>
   <si>
+    <t>Bedingung</t>
+  </si>
+  <si>
+    <t>DK11R</t>
+  </si>
+  <si>
+    <t>HT08S</t>
+  </si>
+  <si>
+    <t>JK12R</t>
+  </si>
+  <si>
+    <t>MS09E</t>
+  </si>
+  <si>
+    <t>MS23B</t>
+  </si>
+  <si>
+    <t>NM11M</t>
+  </si>
+  <si>
+    <t>PA13R</t>
+  </si>
+  <si>
+    <t>SC10R</t>
+  </si>
+  <si>
+    <t>VS09S</t>
+  </si>
+  <si>
+    <t>RM13N</t>
+  </si>
+  <si>
     <t>SK12K</t>
+  </si>
+  <si>
+    <t>SU29N</t>
   </si>
 </sst>
 </file>
@@ -1367,10 +1382,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C6556BD-B14F-40B1-BB2F-75636F2AD0F4}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:B116"/>
+  <dimension ref="A1:B123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D105" sqref="D105"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="400" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1380,60 +1395,60 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>160</v>
       </c>
       <c r="B2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>229</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>257</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>239</v>
       </c>
       <c r="B7">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>258</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -1441,63 +1456,63 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="B9">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>136</v>
+        <v>157</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>151</v>
+        <v>252</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="B12">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>259</v>
       </c>
       <c r="B13">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>163</v>
+        <v>251</v>
       </c>
       <c r="B14">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>172</v>
+        <v>226</v>
       </c>
       <c r="B15">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>175</v>
+        <v>112</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -1505,119 +1520,119 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>210</v>
+        <v>249</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>211</v>
+        <v>188</v>
       </c>
       <c r="B20">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>225</v>
+        <v>187</v>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>226</v>
+        <v>118</v>
       </c>
       <c r="B22">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>228</v>
+        <v>280</v>
       </c>
       <c r="B23">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>234</v>
+        <v>209</v>
       </c>
       <c r="B24">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
       <c r="B25">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>243</v>
+        <v>161</v>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>245</v>
+        <v>263</v>
       </c>
       <c r="B27">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>249</v>
+        <v>207</v>
       </c>
       <c r="B28">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>250</v>
+        <v>217</v>
       </c>
       <c r="B29">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>259</v>
+        <v>221</v>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>261</v>
+        <v>222</v>
       </c>
       <c r="B31">
         <v>3</v>
@@ -1625,71 +1640,71 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>262</v>
+        <v>208</v>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>265</v>
+        <v>243</v>
       </c>
       <c r="B33">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>269</v>
+        <v>101</v>
       </c>
       <c r="B34">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>272</v>
+        <v>216</v>
       </c>
       <c r="B35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>275</v>
+        <v>106</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="B37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>281</v>
       </c>
       <c r="B38">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>201</v>
       </c>
       <c r="B39">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>30</v>
+        <v>278</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -1697,23 +1712,23 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>133</v>
+        <v>241</v>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>49</v>
+        <v>203</v>
       </c>
       <c r="B42">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>193</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -1721,7 +1736,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>59</v>
+        <v>200</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1729,23 +1744,23 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>138</v>
       </c>
       <c r="B45">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>93</v>
+        <v>59</v>
       </c>
       <c r="B46">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>107</v>
+        <v>282</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -1753,15 +1768,15 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>117</v>
+        <v>272</v>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>126</v>
+        <v>103</v>
       </c>
       <c r="B49">
         <v>1</v>
@@ -1769,31 +1784,31 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>132</v>
+        <v>248</v>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>160</v>
+        <v>262</v>
       </c>
       <c r="B51">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>164</v>
+        <v>220</v>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>181</v>
+        <v>234</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -1801,23 +1816,23 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>186</v>
+        <v>242</v>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="B56">
         <v>1</v>
@@ -1825,7 +1840,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>193</v>
+        <v>212</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1833,15 +1848,15 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>205</v>
+        <v>186</v>
       </c>
       <c r="B58">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B59">
         <v>1</v>
@@ -1849,7 +1864,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>216</v>
+        <v>275</v>
       </c>
       <c r="B60">
         <v>1</v>
@@ -1857,7 +1872,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>223</v>
+        <v>107</v>
       </c>
       <c r="B61">
         <v>1</v>
@@ -1865,15 +1880,15 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>237</v>
+        <v>151</v>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>127</v>
+        <v>268</v>
       </c>
       <c r="B63">
         <v>2</v>
@@ -1881,7 +1896,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>248</v>
+        <v>135</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -1889,15 +1904,15 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>264</v>
+        <v>95</v>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>267</v>
+        <v>202</v>
       </c>
       <c r="B66">
         <v>1</v>
@@ -1905,15 +1920,15 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>271</v>
+        <v>206</v>
       </c>
       <c r="B67">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
       <c r="B68">
         <v>1</v>
@@ -1921,7 +1936,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>274</v>
+        <v>224</v>
       </c>
       <c r="B69">
         <v>1</v>
@@ -1929,7 +1944,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>167</v>
+        <v>197</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -1937,39 +1952,39 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>170</v>
+        <v>269</v>
       </c>
       <c r="B71">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>29</v>
+        <v>199</v>
       </c>
       <c r="B72">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>66</v>
+        <v>110</v>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>69</v>
+        <v>195</v>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>95</v>
+        <v>162</v>
       </c>
       <c r="B75">
         <v>2</v>
@@ -1977,7 +1992,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B76">
         <v>2</v>
@@ -1985,7 +2000,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>244</v>
       </c>
       <c r="B77">
         <v>2</v>
@@ -1993,15 +2008,15 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>114</v>
+        <v>270</v>
       </c>
       <c r="B78">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>118</v>
+        <v>277</v>
       </c>
       <c r="B79">
         <v>2</v>
@@ -2009,7 +2024,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>131</v>
+        <v>198</v>
       </c>
       <c r="B80">
         <v>2</v>
@@ -2017,7 +2032,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>140</v>
+        <v>273</v>
       </c>
       <c r="B81">
         <v>2</v>
@@ -2025,15 +2040,15 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>168</v>
+        <v>235</v>
       </c>
       <c r="B82">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="B83">
         <v>2</v>
@@ -2041,15 +2056,15 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>184</v>
+        <v>81</v>
       </c>
       <c r="B84">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>188</v>
+        <v>266</v>
       </c>
       <c r="B85">
         <v>2</v>
@@ -2057,23 +2072,23 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>196</v>
+        <v>265</v>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>201</v>
+        <v>219</v>
       </c>
       <c r="B87">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>204</v>
+        <v>256</v>
       </c>
       <c r="B88">
         <v>2</v>
@@ -2081,7 +2096,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>209</v>
+        <v>228</v>
       </c>
       <c r="B89">
         <v>2</v>
@@ -2089,23 +2104,23 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>213</v>
+        <v>283</v>
       </c>
       <c r="B90">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>214</v>
+        <v>284</v>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>231</v>
+        <v>274</v>
       </c>
       <c r="B92">
         <v>2</v>
@@ -2113,15 +2128,15 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>240</v>
+        <v>285</v>
       </c>
       <c r="B93">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>256</v>
+        <v>183</v>
       </c>
       <c r="B94">
         <v>2</v>
@@ -2129,7 +2144,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>266</v>
+        <v>286</v>
       </c>
       <c r="B95">
         <v>2</v>
@@ -2137,23 +2152,23 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>268</v>
+        <v>39</v>
       </c>
       <c r="B96">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B97">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>277</v>
+        <v>184</v>
       </c>
       <c r="B98">
         <v>2</v>
@@ -2161,7 +2176,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>55</v>
+        <v>214</v>
       </c>
       <c r="B99">
         <v>2</v>
@@ -2169,23 +2184,23 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>139</v>
+        <v>289</v>
       </c>
       <c r="B100">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>141</v>
+        <v>227</v>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>182</v>
+        <v>287</v>
       </c>
       <c r="B102">
         <v>2</v>
@@ -2193,7 +2208,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>235</v>
+        <v>131</v>
       </c>
       <c r="B103">
         <v>2</v>
@@ -2201,7 +2216,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>263</v>
+        <v>276</v>
       </c>
       <c r="B104">
         <v>2</v>
@@ -2209,7 +2224,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>286</v>
+        <v>168</v>
       </c>
       <c r="B105">
         <v>2</v>
@@ -2217,39 +2232,39 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>242</v>
+        <v>290</v>
       </c>
       <c r="B107">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>284</v>
+        <v>69</v>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>279</v>
+        <v>141</v>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>280</v>
+        <v>127</v>
       </c>
       <c r="B110">
         <v>2</v>
@@ -2257,15 +2272,15 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>285</v>
+        <v>190</v>
       </c>
       <c r="B111">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>281</v>
+        <v>247</v>
       </c>
       <c r="B112">
         <v>1</v>
@@ -2273,15 +2288,15 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>282</v>
+        <v>179</v>
       </c>
       <c r="B113">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>283</v>
+        <v>291</v>
       </c>
       <c r="B114">
         <v>1</v>
@@ -2289,22 +2304,77 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>194</v>
+        <v>261</v>
       </c>
       <c r="B115">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>241</v>
+        <v>264</v>
       </c>
       <c r="B116">
-        <v>3</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A117" t="s">
+        <v>218</v>
+      </c>
+      <c r="B117">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A118" t="s">
+        <v>204</v>
+      </c>
+      <c r="B118">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A119" t="s">
+        <v>40</v>
+      </c>
+      <c r="B119">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A120" t="s">
+        <v>260</v>
+      </c>
+      <c r="B120">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A121" t="s">
+        <v>245</v>
+      </c>
+      <c r="B121">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A122" t="s">
+        <v>288</v>
+      </c>
+      <c r="B122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A123" t="s">
+        <v>205</v>
+      </c>
+      <c r="B123">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D107" xr:uid="{3391A0D9-27C3-4DA1-9B17-C54A98E6B964}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>